<commit_message>
Added files for DE441 and DE440
</commit_message>
<xml_diff>
--- a/doc/de441_de440_parameters.xlsx
+++ b/doc/de441_de440_parameters.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottbriggs/Documents/GitHub/computational-astronomy/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4469C5A5-A5D5-8040-99FC-9B2241892B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F33807-97A6-9148-A5FB-D1ED06883737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{FEC0A4D2-784A-3F4D-8F3C-6CD367809BA0}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{FEC0A4D2-784A-3F4D-8F3C-6CD367809BA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DE440" sheetId="3" r:id="rId1"/>
     <sheet name="DE441" sheetId="1" r:id="rId2"/>
+    <sheet name="DE441 Files" sheetId="4" r:id="rId3"/>
+    <sheet name="DE440 Files" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="78">
   <si>
     <t>Body</t>
   </si>
@@ -142,13 +144,142 @@
   </si>
   <si>
     <t>End Epoch: JED = 2688976.5: January 25, 2650: 00:00:00</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Number of Blocks</t>
+  </si>
+  <si>
+    <t>ascm01000</t>
+  </si>
+  <si>
+    <t>ascm02000</t>
+  </si>
+  <si>
+    <t>ascm03000</t>
+  </si>
+  <si>
+    <t>ascm04000</t>
+  </si>
+  <si>
+    <t>ascm05000</t>
+  </si>
+  <si>
+    <t>ascm06000</t>
+  </si>
+  <si>
+    <t>ascm07000</t>
+  </si>
+  <si>
+    <t>ascm08000</t>
+  </si>
+  <si>
+    <t>ascm09000</t>
+  </si>
+  <si>
+    <t>ascm10000</t>
+  </si>
+  <si>
+    <t>ascm11000</t>
+  </si>
+  <si>
+    <t>ascm12000</t>
+  </si>
+  <si>
+    <t>ascm13000</t>
+  </si>
+  <si>
+    <t>ascp00000</t>
+  </si>
+  <si>
+    <t>ascp01000</t>
+  </si>
+  <si>
+    <t>ascp02000</t>
+  </si>
+  <si>
+    <t>ascp03000</t>
+  </si>
+  <si>
+    <t>ascp04000</t>
+  </si>
+  <si>
+    <t>ascp05000</t>
+  </si>
+  <si>
+    <t>ascp06000</t>
+  </si>
+  <si>
+    <t>ascp07000</t>
+  </si>
+  <si>
+    <t>ascp08000</t>
+  </si>
+  <si>
+    <t>ascp09000</t>
+  </si>
+  <si>
+    <t>ascp10000</t>
+  </si>
+  <si>
+    <t>ascp11000</t>
+  </si>
+  <si>
+    <t>ascp12000</t>
+  </si>
+  <si>
+    <t>ascp13000</t>
+  </si>
+  <si>
+    <t>ascp14000</t>
+  </si>
+  <si>
+    <t>ascp15000</t>
+  </si>
+  <si>
+    <t>ascp16000</t>
+  </si>
+  <si>
+    <t>ascp01550</t>
+  </si>
+  <si>
+    <t>ascp01650</t>
+  </si>
+  <si>
+    <t>ascp01750</t>
+  </si>
+  <si>
+    <t>ascp01850</t>
+  </si>
+  <si>
+    <t>ascp01950</t>
+  </si>
+  <si>
+    <t>ascp02050</t>
+  </si>
+  <si>
+    <t>ascp02150</t>
+  </si>
+  <si>
+    <t>ascp02250</t>
+  </si>
+  <si>
+    <t>ascp02350</t>
+  </si>
+  <si>
+    <t>ascp02450</t>
+  </si>
+  <si>
+    <t>ascp02550</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,6 +292,26 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -205,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -215,6 +366,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7EAC12F-3DF5-6340-A4E5-C7AAD1C2005C}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -1325,4 +1479,389 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D043AD3-E3EE-7143-B2BA-1CE10D801FA4}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="6">
+        <v>11414</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="6">
+        <v>11414</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="6">
+        <v>11414</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="7">
+        <v>11415</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E721DC0-AEB1-EA41-8BF3-2D6F685060F2}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1143</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added files file sizes for De441 and DE440
</commit_message>
<xml_diff>
--- a/doc/de441_de440_parameters.xlsx
+++ b/doc/de441_de440_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottbriggs/Documents/GitHub/computational-astronomy/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F33807-97A6-9148-A5FB-D1ED06883737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEE8F6B-E515-F64B-AC0F-8BE12D2765DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{FEC0A4D2-784A-3F4D-8F3C-6CD367809BA0}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="DE441 Files" sheetId="4" r:id="rId3"/>
     <sheet name="DE440 Files" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1093,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7ED4D8-1E5A-F144-AC58-46264BB2520B}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1110,7 +1110,7 @@
     <col min="7" max="7" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1155,8 +1155,12 @@
       <c r="G2" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <f>F2*3*G2</f>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1178,8 +1182,12 @@
       <c r="G3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <f t="shared" ref="I3:I12" si="0">F3*3*G3</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1201,8 +1209,12 @@
       <c r="G4" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1224,8 +1236,12 @@
       <c r="G5" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1247,8 +1263,12 @@
       <c r="G6" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1270,8 +1290,12 @@
       <c r="G7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1293,8 +1317,12 @@
       <c r="G8" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1316,8 +1344,12 @@
       <c r="G9" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1339,8 +1371,12 @@
       <c r="G10" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1362,8 +1398,12 @@
       <c r="G11" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -1385,8 +1425,12 @@
       <c r="G12" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1406,8 +1450,12 @@
       <c r="G13" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <f>F13*2*G13</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -1427,8 +1475,12 @@
       <c r="G14" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <f>F14*3*G14</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -1448,8 +1500,11 @@
       <c r="G15" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -1463,6 +1518,9 @@
         <v>0</v>
       </c>
       <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16">
         <v>0</v>
       </c>
     </row>

</xml_diff>